<commit_message>
edited deck and util
</commit_message>
<xml_diff>
--- a/Example Output.xlsx
+++ b/Example Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jburk\Documents\GitHub\oh_hell\oh_hell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F728CA7A-181A-4B33-8C87-F84FBDBF41F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D9EA0-F7D1-45BB-947F-0EB5BB1D0336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{530F6EF1-25FE-4568-B810-3D0E3594B15E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>each observation is a card played</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>{player1: 14, player2:12}</t>
+  </si>
+  <si>
+    <t>bid_made</t>
   </si>
 </sst>
 </file>
@@ -556,11 +559,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50079B4C-C779-4F48-AA16-DBD5016C4691}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -581,12 +582,12 @@
     <col min="16" max="16" width="8.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -635,8 +636,11 @@
       <c r="P2" t="s">
         <v>9</v>
       </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -683,6 +687,9 @@
         <v>19</v>
       </c>
       <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>